<commit_message>
Made Cone and Cylinder
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20610" windowHeight="12000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15285" windowHeight="3870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
   <si>
     <t>TODO</t>
   </si>
@@ -129,7 +130,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="7">
     <dxf>
       <fill>
         <patternFill>
@@ -151,13 +152,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -168,24 +162,6 @@
           <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <top/>
-      </border>
     </dxf>
     <dxf>
       <fill>
@@ -489,8 +465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -545,11 +521,17 @@
       <c r="A7" t="s">
         <v>3</v>
       </c>
+      <c r="B7" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
+      <c r="B8" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -596,24 +578,24 @@
     </row>
   </sheetData>
   <sortState ref="A2:B11">
-    <sortCondition sortBy="cellColor" ref="B2:B11" dxfId="9"/>
-    <sortCondition descending="1" sortBy="cellColor" ref="B2:B11" dxfId="8"/>
+    <sortCondition sortBy="cellColor" ref="B2:B11" dxfId="6"/>
+    <sortCondition descending="1" sortBy="cellColor" ref="B2:B11" dxfId="5"/>
     <sortCondition ref="A2:A11"/>
-    <sortCondition descending="1" sortBy="cellColor" ref="B2:B11" dxfId="7"/>
+    <sortCondition descending="1" sortBy="cellColor" ref="B2:B11" dxfId="4"/>
   </sortState>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Block">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Block">
       <formula>NOT(ISERROR(SEARCH("Block",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B178">
-    <cfRule type="containsBlanks" dxfId="6" priority="5">
+    <cfRule type="containsBlanks" dxfId="1" priority="5">
       <formula>LEN(TRIM(B2))=0</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="In-Progress">
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="In-Progress">
       <formula>NOT(ISERROR(SEARCH("In-Progress",B2)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>